<commit_message>
Examples 20 and 21 added
</commit_message>
<xml_diff>
--- a/examples-tracking/matlab_examples-global.xlsx
+++ b/examples-tracking/matlab_examples-global.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\costa\Desktop\5.2\Tesi\git\AMC_Model\examples-tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49E6975-3A4E-4EC6-8825-94C8A691313C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F921A2-6556-41C1-A5CE-53A27050B7F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="7980" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{59A096B2-CAF5-49DD-A611-81383B903F68}"/>
+    <workbookView xWindow="-20610" yWindow="7980" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="6" xr2:uid="{59A096B2-CAF5-49DD-A611-81383B903F68}"/>
   </bookViews>
   <sheets>
     <sheet name="n=10,4par" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="101">
   <si>
     <t>A1</t>
   </si>
@@ -314,6 +314,36 @@
   </si>
   <si>
     <t>Size: 32(w)x16</t>
+  </si>
+  <si>
+    <t>ESEMPIO 20</t>
+  </si>
+  <si>
+    <t>Block (64,200)</t>
+  </si>
+  <si>
+    <t>Cur_POC =5</t>
+  </si>
+  <si>
+    <t>Ref_POC=4</t>
+  </si>
+  <si>
+    <t>Size: 64(w)x16</t>
+  </si>
+  <si>
+    <t>ESEMPIO 21</t>
+  </si>
+  <si>
+    <t>Cur_POC =7</t>
+  </si>
+  <si>
+    <t>Ref_POC=6</t>
+  </si>
+  <si>
+    <t>Size: 16(w)x32</t>
+  </si>
+  <si>
+    <t>Block (240,80)</t>
   </si>
 </sst>
 </file>
@@ -400,7 +430,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -415,10 +445,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1268,6 +1294,106 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>152401</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>72841</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>352426</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Immagine 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97E8178A-0F55-4B01-87A6-79823123EDF4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4933951" y="6930841"/>
+          <a:ext cx="5429250" cy="3937183"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>162099</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Immagine 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56388EBA-D4A2-4358-9040-BE51319B2BA5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4838700" y="11982624"/>
+          <a:ext cx="5457825" cy="4419426"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1899,8 +2025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABDEB8DE-3B5F-446A-887E-6DEB4FE5A1BA}">
   <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="D76" sqref="D76"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="G76" sqref="G76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4809,10 +4935,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0EBAA0C-25D4-47E1-813C-3D1223104380}">
-  <dimension ref="A1:H62"/>
+  <dimension ref="A1:H87"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25:E31"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5074,186 +5200,454 @@
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
+      <c r="B37" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="11"/>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
+      <c r="B38" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B39" s="11"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
+      <c r="B39" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B40" s="11"/>
-      <c r="C40" s="11"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
+      <c r="C40" t="s">
+        <v>93</v>
+      </c>
+      <c r="D40" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="11"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B42" s="11"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="11"/>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
-      <c r="E43" s="11"/>
-      <c r="F43" s="11"/>
+      <c r="C41" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B44" s="11"/>
-      <c r="C44" s="11"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="11"/>
+      <c r="C44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B45" s="11"/>
-      <c r="C45" s="11"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
+      <c r="B45" s="6">
+        <v>1</v>
+      </c>
+      <c r="C45" t="s">
+        <v>2</v>
+      </c>
+      <c r="D45">
+        <v>24</v>
+      </c>
+      <c r="E45">
+        <v>-4</v>
+      </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B46" s="11"/>
-      <c r="C46" s="11"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="11"/>
-      <c r="F46" s="11"/>
+      <c r="B46" s="6">
+        <v>2</v>
+      </c>
+      <c r="C46" t="s">
+        <v>3</v>
+      </c>
+      <c r="D46">
+        <v>24</v>
+      </c>
+      <c r="E46">
+        <v>-4</v>
+      </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B47" s="11"/>
-      <c r="C47" s="11"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="11"/>
-      <c r="F47" s="11"/>
+      <c r="B47" s="6">
+        <v>3</v>
+      </c>
+      <c r="C47" t="s">
+        <v>4</v>
+      </c>
+      <c r="D47">
+        <v>24</v>
+      </c>
+      <c r="E47">
+        <v>-4</v>
+      </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B48" s="11"/>
-      <c r="C48" s="11"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="11"/>
-      <c r="F48" s="11"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B49" s="11"/>
-      <c r="C49" s="11"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="11"/>
-      <c r="F49" s="11"/>
+      <c r="B49" s="6">
+        <v>1</v>
+      </c>
+      <c r="C49" t="s">
+        <v>5</v>
+      </c>
+      <c r="D49">
+        <v>118</v>
+      </c>
+      <c r="E49">
+        <v>17</v>
+      </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B50" s="11"/>
-      <c r="C50" s="11"/>
-      <c r="D50" s="11"/>
-      <c r="E50" s="11"/>
-      <c r="F50" s="11"/>
+      <c r="B50" s="6">
+        <v>2</v>
+      </c>
+      <c r="C50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B51" s="11"/>
-      <c r="C51" s="13"/>
-      <c r="D51" s="11"/>
-      <c r="E51" s="11"/>
-      <c r="F51" s="11"/>
+      <c r="C51" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B52" s="11"/>
-      <c r="C52" s="11"/>
-      <c r="D52" s="11"/>
-      <c r="E52" s="11"/>
-      <c r="F52" s="11"/>
+      <c r="B52" s="6">
+        <v>1</v>
+      </c>
+      <c r="C52" t="s">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>22</v>
+      </c>
+      <c r="E52">
+        <v>-3</v>
+      </c>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B53" s="11"/>
-      <c r="C53" s="11"/>
-      <c r="D53" s="11"/>
-      <c r="E53" s="11"/>
-      <c r="F53" s="11"/>
-    </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B54" s="11"/>
-      <c r="C54" s="11"/>
-      <c r="D54" s="11"/>
-      <c r="E54" s="11"/>
-      <c r="F54" s="11"/>
+      <c r="B53" s="6">
+        <v>2</v>
+      </c>
+      <c r="C53" t="s">
+        <v>1</v>
+      </c>
+      <c r="D53">
+        <v>22</v>
+      </c>
+      <c r="E53">
+        <v>-3</v>
+      </c>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B55" s="11"/>
-      <c r="C55" s="11"/>
-      <c r="D55" s="11"/>
-      <c r="E55" s="11"/>
-      <c r="F55" s="11"/>
+      <c r="C55" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D55" s="8"/>
+      <c r="E55" s="8"/>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B56" s="11"/>
-      <c r="C56" s="11"/>
-      <c r="D56" s="12"/>
-      <c r="E56" s="12"/>
+      <c r="C56" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="F56" s="11"/>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B57" s="11"/>
-      <c r="C57" s="11"/>
-      <c r="D57" s="11"/>
-      <c r="E57" s="11"/>
+      <c r="B57" s="6">
+        <v>1</v>
+      </c>
+      <c r="C57" t="s">
+        <v>2</v>
+      </c>
+      <c r="D57">
+        <v>24</v>
+      </c>
+      <c r="E57">
+        <v>-4</v>
+      </c>
       <c r="F57" s="11"/>
     </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B58" s="11"/>
-      <c r="C58" s="11"/>
-      <c r="D58" s="11"/>
-      <c r="E58" s="11"/>
+    <row r="58" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="5"/>
+      <c r="C58" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="F58" s="11"/>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B59" s="11"/>
-      <c r="C59" s="11"/>
-      <c r="D59" s="11"/>
-      <c r="E59" s="11"/>
+      <c r="B59" s="6">
+        <v>2</v>
+      </c>
+      <c r="C59" t="s">
+        <v>6</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
       <c r="F59" s="11"/>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B60" s="11"/>
-      <c r="C60" s="13"/>
+      <c r="C60" s="11"/>
       <c r="D60" s="11"/>
       <c r="E60" s="11"/>
       <c r="F60" s="11"/>
+      <c r="H60" s="11"/>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B61" s="11"/>
-      <c r="C61" s="11"/>
-      <c r="D61" s="11"/>
-      <c r="E61" s="11"/>
-      <c r="F61" s="11"/>
       <c r="H61" s="11"/>
     </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H62" s="11"/>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B63" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C63" s="7"/>
+      <c r="D63" s="7"/>
+      <c r="E63" s="7"/>
+      <c r="F63" s="7"/>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
+        <v>97</v>
+      </c>
+      <c r="D66" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C70" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B71" s="6">
+        <v>1</v>
+      </c>
+      <c r="C71" t="s">
+        <v>2</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B72" s="6">
+        <v>2</v>
+      </c>
+      <c r="C72" t="s">
+        <v>3</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B73" s="6">
+        <v>3</v>
+      </c>
+      <c r="C73" t="s">
+        <v>4</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B74" s="5"/>
+      <c r="C74" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B75" s="6">
+        <v>1</v>
+      </c>
+      <c r="C75" t="s">
+        <v>5</v>
+      </c>
+      <c r="D75">
+        <v>0</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B76" s="6">
+        <v>2</v>
+      </c>
+      <c r="C76" t="s">
+        <v>6</v>
+      </c>
+      <c r="D76">
+        <v>11</v>
+      </c>
+      <c r="E76">
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C77" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B78" s="6">
+        <v>1</v>
+      </c>
+      <c r="C78" t="s">
+        <v>0</v>
+      </c>
+      <c r="D78">
+        <v>-10</v>
+      </c>
+      <c r="E78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B79" s="6">
+        <v>2</v>
+      </c>
+      <c r="C79" t="s">
+        <v>1</v>
+      </c>
+      <c r="D79">
+        <v>0</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C81" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D81" s="8"/>
+      <c r="E81" s="8"/>
+    </row>
+    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C82" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F82" s="11"/>
+    </row>
+    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B83" s="6">
+        <v>1</v>
+      </c>
+      <c r="C83" t="s">
+        <v>2</v>
+      </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
+      <c r="E83">
+        <v>0</v>
+      </c>
+      <c r="F83" s="11"/>
+    </row>
+    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B84" s="5"/>
+      <c r="C84" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F84" s="11"/>
+    </row>
+    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B85" s="6">
+        <v>1</v>
+      </c>
+      <c r="C85" t="s">
+        <v>5</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+      <c r="E85">
+        <v>0</v>
+      </c>
+      <c r="F85" s="11"/>
+    </row>
+    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C86" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B87" s="6">
+        <v>2</v>
+      </c>
+      <c r="C87" t="s">
+        <v>1</v>
+      </c>
+      <c r="D87">
+        <v>0</v>
+      </c>
+      <c r="E87">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Example 25 added and ecample inventory created
</commit_message>
<xml_diff>
--- a/examples-tracking/matlab_examples-global.xlsx
+++ b/examples-tracking/matlab_examples-global.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\costa\Desktop\5.2\Tesi\git\AMC_Model\examples-tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{266E2F71-2674-4C31-A1BC-FF04A19524EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9E0FBBD-445D-4C37-8993-33CE827A4D21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20610" yWindow="7980" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="5" xr2:uid="{59A096B2-CAF5-49DD-A611-81383B903F68}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="107">
   <si>
     <t>A1</t>
   </si>
@@ -350,6 +350,18 @@
   </si>
   <si>
     <t>Block (224,128)</t>
+  </si>
+  <si>
+    <t>ESEMPIO 25</t>
+  </si>
+  <si>
+    <t>Block (16,160)</t>
+  </si>
+  <si>
+    <t>Cur_POC =25</t>
+  </si>
+  <si>
+    <t>*Se vai a vedere proprio il blocco è appilcata la stima con modellazione geometrica (Merge GEO). In un caso del genere ho scelto di prendere il MV indicato in "Selection Info" anziché quello indicato da B0 in sé. (Questo fa s' che la costruzione del blocco sia VTM-Compliant)</t>
   </si>
 </sst>
 </file>
@@ -1345,6 +1357,56 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>45366</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Immagine 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD2CD991-412F-42CD-80AC-9DC4EB598D01}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4772025" y="17952366"/>
+          <a:ext cx="5305425" cy="4564733"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4700,10 +4762,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{451FC1BF-9EF4-43BD-A73C-08EC918EDEA4}">
-  <dimension ref="A1:H90"/>
+  <dimension ref="A1:J121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="H67" sqref="H67"/>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="F116" sqref="F116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5430,6 +5492,238 @@
       </c>
       <c r="E90">
         <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B95" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C95" s="7"/>
+      <c r="D95" s="7"/>
+      <c r="E95" s="7"/>
+      <c r="F95" s="7"/>
+    </row>
+    <row r="96" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C98" t="s">
+        <v>105</v>
+      </c>
+      <c r="D98" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C99" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="102" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C102" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D102" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E102" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="103" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B103" s="6">
+        <v>1</v>
+      </c>
+      <c r="C103" t="s">
+        <v>2</v>
+      </c>
+      <c r="D103">
+        <v>28</v>
+      </c>
+      <c r="E103">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="104" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B104" s="6">
+        <v>2</v>
+      </c>
+      <c r="C104" t="s">
+        <v>3</v>
+      </c>
+      <c r="D104">
+        <v>28</v>
+      </c>
+      <c r="E104">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="105" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B105" s="6">
+        <v>3</v>
+      </c>
+      <c r="C105" t="s">
+        <v>4</v>
+      </c>
+      <c r="D105">
+        <v>40</v>
+      </c>
+      <c r="E105">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="106" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B106" s="5"/>
+      <c r="C106" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="107" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B107" s="6">
+        <v>1</v>
+      </c>
+      <c r="C107" t="s">
+        <v>5</v>
+      </c>
+      <c r="D107">
+        <v>40</v>
+      </c>
+      <c r="E107">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="108" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B108" s="6">
+        <v>2</v>
+      </c>
+      <c r="C108" t="s">
+        <v>6</v>
+      </c>
+      <c r="D108">
+        <v>34</v>
+      </c>
+      <c r="E108">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="109" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C109" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="110" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B110" s="6">
+        <v>1</v>
+      </c>
+      <c r="C110" t="s">
+        <v>0</v>
+      </c>
+      <c r="D110">
+        <v>28</v>
+      </c>
+      <c r="E110">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="111" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B111" s="6">
+        <v>2</v>
+      </c>
+      <c r="C111" t="s">
+        <v>1</v>
+      </c>
+      <c r="D111">
+        <v>15</v>
+      </c>
+      <c r="E111">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="113" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C113" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D113" s="8"/>
+      <c r="E113" s="8"/>
+    </row>
+    <row r="114" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C114" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D114" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E114" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F114" s="11"/>
+    </row>
+    <row r="115" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B115" s="6">
+        <v>3</v>
+      </c>
+      <c r="C115" t="s">
+        <v>4</v>
+      </c>
+      <c r="D115">
+        <v>40</v>
+      </c>
+      <c r="E115">
+        <v>-6</v>
+      </c>
+      <c r="F115" s="11"/>
+    </row>
+    <row r="116" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B116" s="5"/>
+      <c r="C116" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F116" s="11"/>
+    </row>
+    <row r="117" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B117" s="6">
+        <v>1</v>
+      </c>
+      <c r="C117" t="s">
+        <v>5</v>
+      </c>
+      <c r="D117">
+        <v>40</v>
+      </c>
+      <c r="E117">
+        <v>-6</v>
+      </c>
+      <c r="F117" s="11"/>
+    </row>
+    <row r="118" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C118" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="119" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B119" s="6">
+        <v>1</v>
+      </c>
+      <c r="C119" t="s">
+        <v>0</v>
+      </c>
+      <c r="D119">
+        <v>28</v>
+      </c>
+      <c r="E119">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="121" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J121" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Examples 26 and 27 added
</commit_message>
<xml_diff>
--- a/examples-tracking/matlab_examples-global.xlsx
+++ b/examples-tracking/matlab_examples-global.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\costa\Desktop\5.2\Tesi\git\AMC_Model\examples-tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9E0FBBD-445D-4C37-8993-33CE827A4D21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E6948A-FE2C-4A45-85BB-6057C5D31136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="7980" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="5" xr2:uid="{59A096B2-CAF5-49DD-A611-81383B903F68}"/>
+    <workbookView xWindow="-20610" yWindow="7980" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2" xr2:uid="{59A096B2-CAF5-49DD-A611-81383B903F68}"/>
   </bookViews>
   <sheets>
     <sheet name="n=10,4par" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="115">
   <si>
     <t>A1</t>
   </si>
@@ -362,6 +362,30 @@
   </si>
   <si>
     <t>*Se vai a vedere proprio il blocco è appilcata la stima con modellazione geometrica (Merge GEO). In un caso del genere ho scelto di prendere il MV indicato in "Selection Info" anziché quello indicato da B0 in sé. (Questo fa s' che la costruzione del blocco sia VTM-Compliant)</t>
+  </si>
+  <si>
+    <t>ESEMPIO 26</t>
+  </si>
+  <si>
+    <t>Block (32,144)</t>
+  </si>
+  <si>
+    <t>Cur_POC =29</t>
+  </si>
+  <si>
+    <t>Ref_POC=28</t>
+  </si>
+  <si>
+    <t>Size: 16(w)x16</t>
+  </si>
+  <si>
+    <t>ESEMPIO 27</t>
+  </si>
+  <si>
+    <t>Block (192,144)</t>
+  </si>
+  <si>
+    <t>Size: 64x32</t>
   </si>
 </sst>
 </file>
@@ -834,6 +858,56 @@
         <a:xfrm>
           <a:off x="3685763" y="6275830"/>
           <a:ext cx="4886738" cy="3705954"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>579783</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>164496</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>331305</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>64603</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Immagine 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55625422-ABFD-42CD-B1F8-26517EA8D124}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3205370" y="11975496"/>
+          <a:ext cx="4654826" cy="3900607"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1512,6 +1586,56 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>391947</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Immagine 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AAB2FA62-7B91-44FF-BCE2-0DA4E637D1EC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4791075" y="12220575"/>
+          <a:ext cx="5002047" cy="4324350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2699,10 +2823,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28471F49-110A-464B-B794-649FAD3DFDB3}">
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:G86"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N71" sqref="N71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3132,6 +3256,228 @@
       </c>
       <c r="D57">
         <v>-24</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B62" s="7"/>
+      <c r="C62" s="7"/>
+      <c r="D62" s="7"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>40</v>
+      </c>
+      <c r="C65" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B69" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="6">
+        <v>1</v>
+      </c>
+      <c r="B70" t="s">
+        <v>2</v>
+      </c>
+      <c r="C70">
+        <v>97</v>
+      </c>
+      <c r="D70">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="6">
+        <v>2</v>
+      </c>
+      <c r="B71" t="s">
+        <v>3</v>
+      </c>
+      <c r="C71">
+        <v>97</v>
+      </c>
+      <c r="D71">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="6">
+        <v>3</v>
+      </c>
+      <c r="B72" t="s">
+        <v>4</v>
+      </c>
+      <c r="C72">
+        <v>97</v>
+      </c>
+      <c r="D72">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="5"/>
+      <c r="B73" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="6">
+        <v>1</v>
+      </c>
+      <c r="B74" t="s">
+        <v>5</v>
+      </c>
+      <c r="C74">
+        <v>-64</v>
+      </c>
+      <c r="D74">
+        <v>-40</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="6">
+        <v>2</v>
+      </c>
+      <c r="B75" t="s">
+        <v>6</v>
+      </c>
+      <c r="C75">
+        <v>-96</v>
+      </c>
+      <c r="D75">
+        <v>-32</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B76" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="6">
+        <v>1</v>
+      </c>
+      <c r="B77" t="s">
+        <v>0</v>
+      </c>
+      <c r="C77">
+        <v>98</v>
+      </c>
+      <c r="D77">
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="6">
+        <v>2</v>
+      </c>
+      <c r="B78" t="s">
+        <v>1</v>
+      </c>
+      <c r="C78">
+        <v>98</v>
+      </c>
+      <c r="D78">
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B80" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C80" s="8"/>
+      <c r="D80" s="8"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B81" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="6">
+        <v>3</v>
+      </c>
+      <c r="B82" t="s">
+        <v>4</v>
+      </c>
+      <c r="C82">
+        <v>97</v>
+      </c>
+      <c r="D82">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="5"/>
+      <c r="B83" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="6">
+        <v>1</v>
+      </c>
+      <c r="B84" t="s">
+        <v>5</v>
+      </c>
+      <c r="C84">
+        <v>-64</v>
+      </c>
+      <c r="D84">
+        <v>-40</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B85" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="6">
+        <v>1</v>
+      </c>
+      <c r="B86" t="s">
+        <v>0</v>
+      </c>
+      <c r="C86">
+        <v>98</v>
+      </c>
+      <c r="D86">
+        <v>-7</v>
       </c>
     </row>
   </sheetData>
@@ -4764,7 +5110,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{451FC1BF-9EF4-43BD-A73C-08EC918EDEA4}">
   <dimension ref="A1:J121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+    <sheetView topLeftCell="A104" workbookViewId="0">
       <selection activeCell="F116" sqref="F116"/>
     </sheetView>
   </sheetViews>
@@ -5734,10 +6080,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0EBAA0C-25D4-47E1-813C-3D1223104380}">
-  <dimension ref="A1:H61"/>
+  <dimension ref="A1:H86"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63:F87"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="E78" sqref="E78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6217,6 +6563,214 @@
     <row r="61" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H61" s="11"/>
     </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B64" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C64" s="7"/>
+      <c r="D64" s="7"/>
+      <c r="E64" s="7"/>
+      <c r="F64" s="7"/>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
+        <v>109</v>
+      </c>
+      <c r="D67" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C68" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C71" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B72" s="6">
+        <v>1</v>
+      </c>
+      <c r="C72" t="s">
+        <v>2</v>
+      </c>
+      <c r="D72">
+        <v>37</v>
+      </c>
+      <c r="E72">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B73" s="6">
+        <v>2</v>
+      </c>
+      <c r="C73" t="s">
+        <v>3</v>
+      </c>
+      <c r="D73">
+        <v>37</v>
+      </c>
+      <c r="E73">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B74" s="6">
+        <v>3</v>
+      </c>
+      <c r="C74" t="s">
+        <v>4</v>
+      </c>
+      <c r="D74">
+        <v>23</v>
+      </c>
+      <c r="E74">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B75" s="5"/>
+      <c r="C75" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B76" s="6">
+        <v>1</v>
+      </c>
+      <c r="C76" t="s">
+        <v>5</v>
+      </c>
+      <c r="D76">
+        <v>23</v>
+      </c>
+      <c r="E76">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B77" s="6">
+        <v>2</v>
+      </c>
+      <c r="C77" t="s">
+        <v>6</v>
+      </c>
+      <c r="D77">
+        <v>25</v>
+      </c>
+      <c r="E77">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C78" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B79" s="6">
+        <v>1</v>
+      </c>
+      <c r="C79" t="s">
+        <v>0</v>
+      </c>
+      <c r="D79">
+        <v>29</v>
+      </c>
+      <c r="E79">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B80" s="6">
+        <v>2</v>
+      </c>
+      <c r="C80" t="s">
+        <v>1</v>
+      </c>
+      <c r="D80">
+        <v>15</v>
+      </c>
+      <c r="E80">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C82" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D82" s="8"/>
+      <c r="E82" s="8"/>
+    </row>
+    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C83" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D83" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E83" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F83" s="11"/>
+    </row>
+    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B84" s="6">
+        <v>2</v>
+      </c>
+      <c r="C84" t="s">
+        <v>3</v>
+      </c>
+      <c r="D84">
+        <v>37</v>
+      </c>
+      <c r="E84">
+        <v>-6</v>
+      </c>
+      <c r="F84" s="11"/>
+    </row>
+    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B85" s="5"/>
+      <c r="C85" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F85" s="11"/>
+    </row>
+    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B86" s="6">
+        <v>1</v>
+      </c>
+      <c r="C86" t="s">
+        <v>5</v>
+      </c>
+      <c r="D86">
+        <v>23</v>
+      </c>
+      <c r="E86">
+        <v>12</v>
+      </c>
+      <c r="F86" s="11"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Examples 28 and 29 added
</commit_message>
<xml_diff>
--- a/examples-tracking/matlab_examples-global.xlsx
+++ b/examples-tracking/matlab_examples-global.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\costa\Desktop\5.2\Tesi\git\AMC_Model\examples-tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E6948A-FE2C-4A45-85BB-6057C5D31136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4BBB99D-C382-4807-B8F4-D1963F7357D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="7980" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2" xr2:uid="{59A096B2-CAF5-49DD-A611-81383B903F68}"/>
+    <workbookView xWindow="-20610" yWindow="7980" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="6" xr2:uid="{59A096B2-CAF5-49DD-A611-81383B903F68}"/>
   </bookViews>
   <sheets>
     <sheet name="n=10,4par" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="121">
   <si>
     <t>A1</t>
   </si>
@@ -386,6 +386,24 @@
   </si>
   <si>
     <t>Size: 64x32</t>
+  </si>
+  <si>
+    <t>ESEMPIO 28</t>
+  </si>
+  <si>
+    <t>Block (136,168)</t>
+  </si>
+  <si>
+    <t>ESEMPIO 29</t>
+  </si>
+  <si>
+    <t>Block (264,96)</t>
+  </si>
+  <si>
+    <t>Cur_POC =38</t>
+  </si>
+  <si>
+    <t>Ref_POC=37</t>
   </si>
 </sst>
 </file>
@@ -753,6 +771,56 @@
         <a:xfrm>
           <a:off x="3467101" y="9548794"/>
           <a:ext cx="5734050" cy="3805256"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>6399</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Immagine 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC6F173C-332D-469E-8C97-8920A70DBDA3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3409950" y="15246399"/>
+          <a:ext cx="5486400" cy="4441776"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1636,6 +1704,56 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>429801</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>16517</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Immagine 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5EE7465B-8292-4C20-8FE7-0A3B47FB1036}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4619625" y="17430749"/>
+          <a:ext cx="5211351" cy="4312293"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2265,10 +2383,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABDEB8DE-3B5F-446A-887E-6DEB4FE5A1BA}">
-  <dimension ref="A1:D73"/>
+  <dimension ref="A1:D103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G76" sqref="G76"/>
+    <sheetView topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="E101" sqref="E101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2815,6 +2933,209 @@
         <v>29</v>
       </c>
     </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B80" s="7"/>
+      <c r="C80" s="7"/>
+      <c r="D80" s="7"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>18</v>
+      </c>
+      <c r="C83" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B87" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D87" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="6">
+        <v>1</v>
+      </c>
+      <c r="B88" t="s">
+        <v>2</v>
+      </c>
+      <c r="C88">
+        <v>88</v>
+      </c>
+      <c r="D88">
+        <v>-24</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="6">
+        <v>2</v>
+      </c>
+      <c r="B89" t="s">
+        <v>3</v>
+      </c>
+      <c r="C89">
+        <v>88</v>
+      </c>
+      <c r="D89">
+        <v>-24</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="6">
+        <v>3</v>
+      </c>
+      <c r="B90" t="s">
+        <v>4</v>
+      </c>
+      <c r="C90">
+        <v>102</v>
+      </c>
+      <c r="D90">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="5"/>
+      <c r="B91" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="6">
+        <v>1</v>
+      </c>
+      <c r="B92" t="s">
+        <v>5</v>
+      </c>
+      <c r="C92">
+        <v>103</v>
+      </c>
+      <c r="D92">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="6">
+        <v>2</v>
+      </c>
+      <c r="B93" t="s">
+        <v>6</v>
+      </c>
+      <c r="C93">
+        <v>112</v>
+      </c>
+      <c r="D93">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B94" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="6">
+        <v>1</v>
+      </c>
+      <c r="B95" t="s">
+        <v>0</v>
+      </c>
+      <c r="C95">
+        <v>88</v>
+      </c>
+      <c r="D95">
+        <v>-24</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="6">
+        <v>2</v>
+      </c>
+      <c r="B96" t="s">
+        <v>1</v>
+      </c>
+      <c r="C96">
+        <v>88</v>
+      </c>
+      <c r="D96">
+        <v>-24</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B99" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C99" s="8"/>
+      <c r="D99" s="8"/>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B100" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C100" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D100" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="6">
+        <v>3</v>
+      </c>
+      <c r="B101" t="s">
+        <v>4</v>
+      </c>
+      <c r="C101">
+        <v>102</v>
+      </c>
+      <c r="D101">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="5"/>
+      <c r="B102" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="6">
+        <v>1</v>
+      </c>
+      <c r="B103" t="s">
+        <v>5</v>
+      </c>
+      <c r="C103">
+        <v>103</v>
+      </c>
+      <c r="D103">
+        <v>-9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2825,8 +3146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28471F49-110A-464B-B794-649FAD3DFDB3}">
   <dimension ref="A1:G86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N71" sqref="N71"/>
+    <sheetView topLeftCell="A71" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3490,8 +3811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65113F10-061B-4B09-B2DF-139F685758A8}">
   <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="Q70" sqref="Q70"/>
+    <sheetView topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58:D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6080,10 +6401,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0EBAA0C-25D4-47E1-813C-3D1223104380}">
-  <dimension ref="A1:H86"/>
+  <dimension ref="A1:H113"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="E78" sqref="E78"/>
+    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="D115" sqref="D115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6771,6 +7092,214 @@
       </c>
       <c r="F86" s="11"/>
     </row>
+    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B91" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C91" s="7"/>
+      <c r="D91" s="7"/>
+      <c r="E91" s="7"/>
+      <c r="F91" s="7"/>
+    </row>
+    <row r="92" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="94" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C94" t="s">
+        <v>119</v>
+      </c>
+      <c r="D94" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C95" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="98" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C98" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D98" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E98" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="99" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B99" s="6">
+        <v>1</v>
+      </c>
+      <c r="C99" t="s">
+        <v>2</v>
+      </c>
+      <c r="D99">
+        <v>-4</v>
+      </c>
+      <c r="E99">
+        <v>-24</v>
+      </c>
+    </row>
+    <row r="100" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B100" s="6">
+        <v>2</v>
+      </c>
+      <c r="C100" t="s">
+        <v>3</v>
+      </c>
+      <c r="D100">
+        <v>21</v>
+      </c>
+      <c r="E100">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B101" s="6">
+        <v>3</v>
+      </c>
+      <c r="C101" t="s">
+        <v>4</v>
+      </c>
+      <c r="D101">
+        <v>21</v>
+      </c>
+      <c r="E101">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="102" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B102" s="5"/>
+      <c r="C102" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="103" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B103" s="6">
+        <v>1</v>
+      </c>
+      <c r="C103" t="s">
+        <v>5</v>
+      </c>
+      <c r="D103">
+        <v>25</v>
+      </c>
+      <c r="E103">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="104" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B104" s="6">
+        <v>2</v>
+      </c>
+      <c r="C104" t="s">
+        <v>6</v>
+      </c>
+      <c r="D104">
+        <v>32</v>
+      </c>
+      <c r="E104">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="105" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C105" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="106" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B106" s="6">
+        <v>1</v>
+      </c>
+      <c r="C106" t="s">
+        <v>0</v>
+      </c>
+      <c r="D106">
+        <v>-4</v>
+      </c>
+      <c r="E106">
+        <v>-24</v>
+      </c>
+    </row>
+    <row r="107" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B107" s="6">
+        <v>2</v>
+      </c>
+      <c r="C107" t="s">
+        <v>1</v>
+      </c>
+      <c r="D107">
+        <v>0</v>
+      </c>
+      <c r="E107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C109" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D109" s="8"/>
+      <c r="E109" s="8"/>
+    </row>
+    <row r="110" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C110" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D110" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E110" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F110" s="11"/>
+    </row>
+    <row r="111" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B111" s="6">
+        <v>1</v>
+      </c>
+      <c r="C111" t="s">
+        <v>2</v>
+      </c>
+      <c r="D111">
+        <v>-4</v>
+      </c>
+      <c r="E111">
+        <v>-24</v>
+      </c>
+      <c r="F111" s="11"/>
+    </row>
+    <row r="112" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B112" s="5"/>
+      <c r="C112" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F112" s="11"/>
+    </row>
+    <row r="113" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B113" s="6">
+        <v>1</v>
+      </c>
+      <c r="C113" t="s">
+        <v>5</v>
+      </c>
+      <c r="D113">
+        <v>25</v>
+      </c>
+      <c r="E113">
+        <v>-3</v>
+      </c>
+      <c r="F113" s="11"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added examples 30 to 32 and model corrected
</commit_message>
<xml_diff>
--- a/examples-tracking/matlab_examples-global.xlsx
+++ b/examples-tracking/matlab_examples-global.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\costa\Desktop\5.2\Tesi\git\AMC_Model\examples-tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{610F7396-50F8-4ABE-8DCF-5E16A02DB559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C9A4DA-5DD8-4477-B3F9-5280E8A87B54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3735" yWindow="5295" windowWidth="15375" windowHeight="8475" firstSheet="4" activeTab="6" xr2:uid="{59A096B2-CAF5-49DD-A611-81383B903F68}"/>
+    <workbookView xWindow="-20610" yWindow="7980" windowWidth="20730" windowHeight="11040" firstSheet="3" activeTab="6" xr2:uid="{59A096B2-CAF5-49DD-A611-81383B903F68}"/>
   </bookViews>
   <sheets>
     <sheet name="n=10,4par" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="131">
   <si>
     <t>A1</t>
   </si>
@@ -419,6 +419,21 @@
   </si>
   <si>
     <t>Niente da costruire</t>
+  </si>
+  <si>
+    <t>ESEMPIO 31</t>
+  </si>
+  <si>
+    <t>Block (64,64)</t>
+  </si>
+  <si>
+    <t>Cur_POC =4</t>
+  </si>
+  <si>
+    <t>Ref_POC=3</t>
+  </si>
+  <si>
+    <t>Size: 16(w)x64</t>
   </si>
 </sst>
 </file>
@@ -1769,6 +1784,56 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>96074</xdr:colOff>
+      <xdr:row>143</xdr:row>
+      <xdr:rowOff>153041</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Immagine 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83D414E5-5D35-6B59-F433-217EE60D1923}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4810125" y="22812375"/>
+          <a:ext cx="5906324" cy="4591691"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3826,7 +3891,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65113F10-061B-4B09-B2DF-139F685758A8}">
   <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
@@ -6397,10 +6462,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0EBAA0C-25D4-47E1-813C-3D1223104380}">
-  <dimension ref="A1:H113"/>
+  <dimension ref="A1:H143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="G140" sqref="G140"/>
+    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
+      <selection activeCell="B143" sqref="B143:E143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7296,6 +7361,214 @@
       </c>
       <c r="F113" s="11"/>
     </row>
+    <row r="121" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B121" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C121" s="7"/>
+      <c r="D121" s="7"/>
+      <c r="E121" s="7"/>
+      <c r="F121" s="7"/>
+    </row>
+    <row r="122" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B122" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="123" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B123" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="124" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C124" t="s">
+        <v>128</v>
+      </c>
+      <c r="D124" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="125" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C125" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="128" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C128" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D128" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E128" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="129" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B129" s="6">
+        <v>1</v>
+      </c>
+      <c r="C129" t="s">
+        <v>2</v>
+      </c>
+      <c r="D129">
+        <v>32</v>
+      </c>
+      <c r="E129">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="130" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B130" s="6">
+        <v>2</v>
+      </c>
+      <c r="C130" t="s">
+        <v>3</v>
+      </c>
+      <c r="D130">
+        <v>32</v>
+      </c>
+      <c r="E130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B131" s="6">
+        <v>3</v>
+      </c>
+      <c r="C131" t="s">
+        <v>4</v>
+      </c>
+      <c r="D131">
+        <v>32</v>
+      </c>
+      <c r="E131">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="132" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B132" s="5"/>
+      <c r="C132" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="133" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B133" s="6">
+        <v>1</v>
+      </c>
+      <c r="C133" t="s">
+        <v>5</v>
+      </c>
+      <c r="D133">
+        <v>32</v>
+      </c>
+      <c r="E133">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="134" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B134" s="6">
+        <v>2</v>
+      </c>
+      <c r="C134" t="s">
+        <v>6</v>
+      </c>
+      <c r="D134">
+        <v>32</v>
+      </c>
+      <c r="E134">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="135" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C135" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="136" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B136" s="6">
+        <v>1</v>
+      </c>
+      <c r="C136" t="s">
+        <v>0</v>
+      </c>
+      <c r="D136">
+        <v>32</v>
+      </c>
+      <c r="E136">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="137" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B137" s="6">
+        <v>2</v>
+      </c>
+      <c r="C137" t="s">
+        <v>1</v>
+      </c>
+      <c r="D137">
+        <v>32</v>
+      </c>
+      <c r="E137">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="139" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C139" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D139" s="8"/>
+      <c r="E139" s="8"/>
+    </row>
+    <row r="140" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C140" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D140" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E140" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F140" s="11"/>
+    </row>
+    <row r="141" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B141" s="6">
+        <v>1</v>
+      </c>
+      <c r="C141" t="s">
+        <v>2</v>
+      </c>
+      <c r="D141">
+        <v>32</v>
+      </c>
+      <c r="E141">
+        <v>8</v>
+      </c>
+      <c r="F141" s="11"/>
+    </row>
+    <row r="142" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B142" s="5"/>
+      <c r="C142" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F142" s="11"/>
+    </row>
+    <row r="143" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B143" s="6">
+        <v>1</v>
+      </c>
+      <c r="C143" t="s">
+        <v>5</v>
+      </c>
+      <c r="D143">
+        <v>32</v>
+      </c>
+      <c r="E143">
+        <v>8</v>
+      </c>
+      <c r="F143" s="11"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>